<commit_message>
UPDATE: Import & others improvements
</commit_message>
<xml_diff>
--- a/Master Data Karyawan Per 9 Sep 2024.xlsx
+++ b/Master Data Karyawan Per 9 Sep 2024.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__JOB PROJECT__\__JOB__\RSKI\backend-api-web\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6D6AF6-4BB3-4A42-881B-C2ED6431CA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master Data Karyawan" sheetId="1" r:id="rId1"/>
@@ -6934,7 +6940,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7470,6 +7476,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -7517,7 +7526,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7550,9 +7559,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7585,6 +7611,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7760,11 +7803,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB761"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7778,7 +7821,7 @@
     <col min="7" max="7" width="114.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.85546875" customWidth="1"/>
     <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
@@ -7791,7 +7834,7 @@
     <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.28515625" customWidth="1"/>
     <col min="25" max="25" width="34" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="17" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="25.28515625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
UPDATE: Improvement for import karyawans and tgl_diangkat on create update karyawan
</commit_message>
<xml_diff>
--- a/Master Data Karyawan Per 9 Sep 2024.xlsx
+++ b/Master Data Karyawan Per 9 Sep 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__JOB PROJECT__\__JOB__\RSKI\backend-api-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6D6AF6-4BB3-4A42-881B-C2ED6431CA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0E1397-51F7-4D6C-8703-57968F8C4A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7806,8 +7806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB761"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7817,12 +7817,12 @@
     <col min="3" max="3" width="45" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="114.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.85546875" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
@@ -66692,6 +66692,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>